<commit_message>
Exported MN files and fixed few areas with errors. Placedholder data for MPCbS and MN data for BPMCCS
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BEEAE5-E5AE-4FA8-BD01-523BFE663128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89927AC9-6C74-4B96-B011-B1F3D3363FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="255" windowWidth="21210" windowHeight="16395" tabRatio="698" xr2:uid="{26206BE0-D423-40C5-BC54-AB75C15D3AEF}"/>
+    <workbookView xWindow="2070" yWindow="2670" windowWidth="25665" windowHeight="13515" tabRatio="698" xr2:uid="{26206BE0-D423-40C5-BC54-AB75C15D3AEF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="GRA-regularspending" sheetId="2" r:id="rId2"/>
-    <sheet name="GRA-deficitspending" sheetId="3" r:id="rId3"/>
-    <sheet name="GRA-householdtaxes" sheetId="4" r:id="rId4"/>
-    <sheet name="GRA-payrolltaxes" sheetId="5" r:id="rId5"/>
-    <sheet name="GRA-corpincometaxes" sheetId="6" r:id="rId6"/>
+    <sheet name="Set Values Here" sheetId="7" r:id="rId2"/>
+    <sheet name="GRA-carbontax" sheetId="8" r:id="rId3"/>
+    <sheet name="GRA-fueltax" sheetId="9" r:id="rId4"/>
+    <sheet name="GRA-evsubsidy" sheetId="10" r:id="rId5"/>
+    <sheet name="GRA-elecgensubsidy" sheetId="11" r:id="rId6"/>
+    <sheet name="GRA-eleccapconstsubsidy" sheetId="12" r:id="rId7"/>
+    <sheet name="GRA-distsolarsubsidy" sheetId="13" r:id="rId8"/>
+    <sheet name="GRA-fuelsubsidy" sheetId="14" r:id="rId9"/>
+    <sheet name="GRA-ntnldebtinterest" sheetId="15" r:id="rId10"/>
+    <sheet name="GRA-remainder" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +42,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4F81BCB5-E56D-426A-91DB-BCF0877CB817}</author>
+  </authors>
+  <commentList>
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{4F81BCB5-E56D-426A-91DB-BCF0877CB817}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    It is recommended to leave this cell set to zero and to set a non-zero value in at least one other cell in this row.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
   <si>
     <t>GRA Government Revenue Accounting</t>
   </si>
@@ -109,27 +132,15 @@
     <t>Weights do not need to sum to 10.  For example, [0, 3, 5, 5, 7] is a valid set of weights</t>
   </si>
   <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Unit: dimensionless (relative weight)</t>
   </si>
   <si>
-    <t>Change in spending on regular government programs</t>
-  </si>
-  <si>
     <t>none needed</t>
   </si>
   <si>
-    <t>Revenue handling is one of the design decisions a model user should make</t>
-  </si>
-  <si>
     <t>when designing a policy package.</t>
   </si>
   <si>
-    <t>Change in payroll taxes</t>
-  </si>
-  <si>
     <t>use integer values, reflecting the step size of these levers in the web app.</t>
   </si>
   <si>
@@ -152,13 +163,109 @@
   </si>
   <si>
     <t>How To Assign Weights</t>
+  </si>
+  <si>
+    <t>remainder</t>
+  </si>
+  <si>
+    <t>carbon tax revenue</t>
+  </si>
+  <si>
+    <t>fuel tax revenue</t>
+  </si>
+  <si>
+    <t>EV subsidy</t>
+  </si>
+  <si>
+    <t>elec gen subsidy</t>
+  </si>
+  <si>
+    <t>elec cap construction subsidy</t>
+  </si>
+  <si>
+    <t>distributed solar subsidy</t>
+  </si>
+  <si>
+    <t>fuel subsidy</t>
+  </si>
+  <si>
+    <t>national debt interest</t>
+  </si>
+  <si>
+    <t>These levers need to be split into five variables (not subscripts of one variable) in order to</t>
+  </si>
+  <si>
+    <t>allow separate policy implementation schedules for each lever.  However, it's easiest to</t>
+  </si>
+  <si>
+    <t>set the priorities when they are all visible on one sheet.  Therefore, set the priorities on</t>
+  </si>
+  <si>
+    <t>Government Cash Flow Type</t>
+  </si>
+  <si>
+    <t>Regular Spending</t>
+  </si>
+  <si>
+    <t>Deficit Spending</t>
+  </si>
+  <si>
+    <t>Household Taxes</t>
+  </si>
+  <si>
+    <t>Payroll Taxes</t>
+  </si>
+  <si>
+    <t>Set weights below.  Use only integers from 0 to 10.</t>
+  </si>
+  <si>
+    <t>Percentages of Govt Cash Flow Changes Handled via Each Mechanism</t>
+  </si>
+  <si>
+    <t>This is only to help you set weights correctly.  Do not edit the formulas below.  Edit the weights above.</t>
+  </si>
+  <si>
+    <t>this sheet, and the blue tabs read the priorities from this sheet.</t>
+  </si>
+  <si>
+    <t>Government Cash Flow Types</t>
+  </si>
+  <si>
+    <t>The EPS allows the government revenue accounting levers to be set to different values for</t>
+  </si>
+  <si>
+    <t>different sources of government cash flow change.  Each tax or subsidy policy, changes in payments</t>
+  </si>
+  <si>
+    <t>on interest on the national debt, and "remainder" (referring to all other sources of government</t>
+  </si>
+  <si>
+    <t>cash flow change) can each have their own custom weights for each revenue accounting mechanism</t>
+  </si>
+  <si>
+    <t>lever.</t>
+  </si>
+  <si>
+    <t>It is recommended that you avoid using the "deficit spending" mechanism to handle "national debt</t>
+  </si>
+  <si>
+    <t>interest" to avoid creating a feedback loop where deficit spending increases debt, which increases</t>
+  </si>
+  <si>
+    <t>interest, which further increases debt, etc.</t>
+  </si>
+  <si>
+    <t>Corporate Taxes</t>
+  </si>
+  <si>
+    <t>Government revenue handling is one of the design decisions a model user should make</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,8 +289,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +322,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,27 +359,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,6 +399,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jeffrey Rissman" id="{B752AA03-E7FD-47E9-A7F9-587DA10781FB}" userId="S::jeff@energyinnovation.onmicrosoft.com::f3f117cb-d7f5-455c-900f-329d977050a0" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,9 +702,17 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C15" dT="2020-08-18T18:45:50.17" personId="{B752AA03-E7FD-47E9-A7F9-587DA10781FB}" id="{4F81BCB5-E56D-426A-91DB-BCF0877CB817}">
+    <text>It is recommended to leave this cell set to zero and to set a non-zero value in at least one other cell in this row.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3857EE15-0702-4D02-88A1-477DCCE329DB}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -557,17 +731,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -666,10 +840,10 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="7"/>
+      <c r="A26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -678,12 +852,12 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -693,42 +867,88 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="13"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -737,12 +957,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5701521-9FC2-4042-98E9-E9BBB10DD961}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57F2C9C-1694-4A27-BF05-C8B0A1B522A6}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -753,18 +973,51 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B15:F15)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -772,12 +1025,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C50B4E-FBF2-444D-BD05-E8B8FF16BB8D}">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521CDC7A-C360-4D48-B6EF-82826DA4B3B6}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -788,18 +1041,51 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
+      <c r="A2" t="s">
+        <v>47</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B16:F16)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -807,12 +1093,524 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A68863B-602B-4AA3-9BB1-5FE420F9C6BF}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2A49CB-6D0E-4B96-B95B-51D10E021D04}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="6" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="10">
+        <f>IFERROR(B8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="10">
+        <f t="shared" ref="C22:F22" si="0">IFERROR(C8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="10">
+        <f t="shared" ref="B23:F23" si="1">IFERROR(B9/SUM($B9:$F9),1/COUNT($B9:$F9))</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="10">
+        <f t="shared" ref="B24:F24" si="2">IFERROR(B10/SUM($B10:$F10),1/COUNT($B10:$F10))</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="10">
+        <f t="shared" ref="B25:F25" si="3">IFERROR(B11/SUM($B11:$F11),1/COUNT($B11:$F11))</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D25" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="10">
+        <f t="shared" ref="B26:F26" si="4">IFERROR(B12/SUM($B12:$F12),1/COUNT($B12:$F12))</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="10">
+        <f t="shared" ref="B27:F27" si="5">IFERROR(B13/SUM($B13:$F13),1/COUNT($B13:$F13))</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="10">
+        <f t="shared" ref="B28:F28" si="6">IFERROR(B14/SUM($B14:$F14),1/COUNT($B14:$F14))</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="10">
+        <f t="shared" ref="B29:F29" si="7">IFERROR(B15/SUM($B15:$F15),1/COUNT($B15:$F15))</f>
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="10">
+        <f t="shared" ref="B30:F30" si="8">IFERROR(B16/SUM($B16:$F16),1/COUNT($B16:$F16))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C30" s="10">
+        <f t="shared" si="8"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="8"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AF1F77-591B-419B-91FC-2618E46BD93A}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -823,18 +1621,51 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -842,12 +1673,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BAD4D-0026-4619-B04A-40E2C46F2EE8}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3C2F6F-98F7-47BF-A121-519530665716}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -858,17 +1689,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>29</v>
+      <c r="A2" t="s">
+        <v>47</v>
       </c>
       <c r="B2">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B9:F9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
     </row>
@@ -877,12 +1741,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71BD46C-6095-4FC9-BFCD-1D04487E7DB5}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95D8AB2-6798-43D7-AB4D-CF9027D5D76D}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -893,17 +1757,322 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>16</v>
+      <c r="A2" t="s">
+        <v>47</v>
       </c>
       <c r="B2">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B10:F10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB851FAA-54C9-43D6-9286-3EB2FEDE6F50}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B11:F11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A3B53A-6256-48D4-9FF6-54DB202AB422}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B12:F12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB629B-80DD-4A77-AF4C-E5418F20EE0D}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B13:F13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85184EB0-77F4-492B-91CC-4F8870FED453}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B14:F14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
     </row>

</xml_diff>